<commit_message>
Added BO TESTING WITH CSV
</commit_message>
<xml_diff>
--- a/testData/TestCases.xlsx
+++ b/testData/TestCases.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAYP-RealEditor\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B240E2-5C39-4B57-B57A-21C4F167BC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="BOTesting" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +25,138 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TestFile</t>
+  </si>
+  <si>
+    <t>File@123</t>
+  </si>
+  <si>
+    <t>UpdatedFile</t>
+  </si>
+  <si>
+    <t>NonExistentFile</t>
+  </si>
+  <si>
+    <t>TestFileToDelete</t>
+  </si>
+  <si>
+    <t>FileForGetTest</t>
+  </si>
+  <si>
+    <t>FileToUpdate</t>
+  </si>
+  <si>
+    <t>TransliterationTestFile</t>
+  </si>
+  <si>
+    <t>This is a test content.</t>
+  </si>
+  <si>
+    <t>Updated content.</t>
+  </si>
+  <si>
+    <t>Some content.</t>
+  </si>
+  <si>
+    <t>Content for deletion</t>
+  </si>
+  <si>
+    <t>Content to retrieve</t>
+  </si>
+  <si>
+    <t>مرحبا</t>
+  </si>
+  <si>
+    <t>A (repeated 1024*1024 times)</t>
+  </si>
+  <si>
+    <t>MrHba</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +179,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +467,468 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{5A993E1B-93B3-4A6A-A5A7-6896A0A90791}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCA8356-E3DB-4047-9FA0-22AFFEF2F854}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{FB5EC7EE-7C6B-4DB3-9FD0-85BC70496F7A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added excel and edited test cases
</commit_message>
<xml_diff>
--- a/testData/TestCases.xlsx
+++ b/testData/TestCases.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\5th Sem\SQE\LAYP-RealEditor\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FBD355-4856-4208-9D6B-FF9709014507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,138 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TestFile</t>
+  </si>
+  <si>
+    <t>File@123</t>
+  </si>
+  <si>
+    <t>UpdatedFile</t>
+  </si>
+  <si>
+    <t>NonExistentFile</t>
+  </si>
+  <si>
+    <t>TestFileToDelete</t>
+  </si>
+  <si>
+    <t>FileForGetTest</t>
+  </si>
+  <si>
+    <t>FileToUpdate</t>
+  </si>
+  <si>
+    <t>TransliterationTestFile</t>
+  </si>
+  <si>
+    <t>This is a test content.</t>
+  </si>
+  <si>
+    <t>Updated content.</t>
+  </si>
+  <si>
+    <t>Some content.</t>
+  </si>
+  <si>
+    <t>Content for deletion</t>
+  </si>
+  <si>
+    <t>Content to retrieve</t>
+  </si>
+  <si>
+    <t>مرحبا</t>
+  </si>
+  <si>
+    <t>A (repeated 1024*1024 times)</t>
+  </si>
+  <si>
+    <t>MrHba</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +178,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +466,238 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{5A993E1B-93B3-4A6A-A5A7-6896A0A90791}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>